<commit_message>
Trình diễn dữ liệu PhuLuc01 tiến độ 50%
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/bcTuan_PL.xlsx
+++ b/ToolBaoCao/App_Data/bcTuan_PL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7874F503-17F2-43AF-ADB5-ED98E442F87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0E06EB-FF71-405F-BEF4-23EC06127F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9C48385-093D-48CA-9E2E-0D4867CB3FBE}"/>
   </bookViews>
@@ -134,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -142,7 +142,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,7 +459,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -514,7 +513,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>